<commit_message>
resoved the null pointer exception
</commit_message>
<xml_diff>
--- a/src/main/resources/Book1.xlsx
+++ b/src/main/resources/Book1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">User01808@yopmail.com</t>
   </si>
@@ -28,7 +28,19 @@
     <t xml:space="preserve">abcd</t>
   </si>
   <si>
-    <t>User0185@yopmail.com</t>
+    <t xml:space="preserve">User0185@yopmail.com</t>
+  </si>
+  <si>
+    <t>User0224@yopmail.com</t>
+  </si>
+  <si>
+    <t>User02880@yopmail.com</t>
+  </si>
+  <si>
+    <t>User01329@yopmail.com</t>
+  </si>
+  <si>
+    <t>User0721@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -105,7 +117,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -115,10 +127,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -141,8 +149,8 @@
   </sheetPr>
   <dimension ref="B1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A473" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B517" activeCellId="0" sqref="B517"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -161,18 +169,38 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="0"/>
+    </row>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
updated the script to get pcid and store it in the excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/Book1.xlsx
+++ b/src/main/resources/Book1.xlsx
@@ -20,27 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">User01808@yopmail.com</t>
+    <t xml:space="preserve">TestUserForPerf5355@yopmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">abcd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User0185@yopmail.com</t>
-  </si>
-  <si>
-    <t>User0224@yopmail.com</t>
-  </si>
-  <si>
-    <t>User02880@yopmail.com</t>
-  </si>
-  <si>
-    <t>User01329@yopmail.com</t>
-  </si>
-  <si>
-    <t>User0721@yopmail.com</t>
+    <t xml:space="preserve">d5ea6bd4-cb26-4dc3-a837-03c0b3c1a78f</t>
   </si>
 </sst>
 </file>
@@ -117,16 +102,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -147,55 +128,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:C8"/>
+  <dimension ref="B1:C1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A473" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B517" activeCellId="0" sqref="B517"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="false" hidden="false" style="1" width="8.54" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="23.15" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="1024" customWidth="false" hidden="false" style="1" width="8.54" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="52.91"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="0"/>
-    </row>
-    <row r="3">
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
updated the script to avoid duplicate entries in the sheet and fix the my account flow
</commit_message>
<xml_diff>
--- a/src/main/resources/Book1.xlsx
+++ b/src/main/resources/Book1.xlsx
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">TestUserForPerf5355@yopmail.com</t>
+    <t>TestUserForPerf923731@yopmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">d5ea6bd4-cb26-4dc3-a837-03c0b3c1a78f</t>
+    <t>327c767a-1893-457b-8123-195bfc175795</t>
+  </si>
+  <si>
+    <t>TestUserForPerf130748@yopmail.com</t>
+  </si>
+  <si>
+    <t>2a52afba-e1d1-4332-9fa6-6218a6fa197a</t>
   </si>
 </sst>
 </file>
@@ -128,26 +134,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:C1"/>
+  <dimension ref="B1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="52.91"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="8.54"/>
+    <col min="1" max="1" customWidth="false" hidden="false" style="1" width="8.54" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="35.28" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="52.91" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="1024" customWidth="false" hidden="false" style="1" width="8.54" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>